<commit_message>
Fixed networking with less balls
</commit_message>
<xml_diff>
--- a/08024 Mark Scheme 16-17.xlsx
+++ b/08024 Mark Scheme 16-17.xlsx
@@ -836,10 +836,10 @@
   <dimension ref="A1:V56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C37" sqref="C37"/>
+      <selection pane="bottomRight" activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -935,7 +935,7 @@
       </c>
       <c r="C4" s="26">
         <f t="shared" ref="C4" si="0">SUMPRODUCT($B5:$B12,C5:C12)/SUM($B5:$B12)/10</f>
-        <v>0.96250000000000002</v>
+        <v>0.95</v>
       </c>
       <c r="D4" s="26"/>
       <c r="E4" s="26"/>
@@ -1115,7 +1115,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="30">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" s="30"/>
       <c r="E10" s="30"/>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="C14" s="26">
         <f t="shared" ref="C14" si="1">SUMPRODUCT($B15:$B18,C15:C18)/SUM($B15:$B18)/10</f>
-        <v>0.9</v>
+        <v>0.6</v>
       </c>
       <c r="D14" s="26"/>
       <c r="E14" s="26"/>
@@ -1259,7 +1259,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="30">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D15" s="30"/>
       <c r="E15" s="30"/>
@@ -1349,7 +1349,7 @@
         <v>1</v>
       </c>
       <c r="C18" s="30">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D18" s="30"/>
       <c r="E18" s="30"/>
@@ -1405,7 +1405,7 @@
       </c>
       <c r="C20" s="28">
         <f t="shared" ref="C20" si="2">((C4*$B4)+(C14*$B14))/$B20</f>
-        <v>0.93125000000000013</v>
+        <v>0.77499999999999991</v>
       </c>
       <c r="D20" s="28"/>
       <c r="E20" s="28"/>
@@ -1484,7 +1484,7 @@
       </c>
       <c r="C23" s="26">
         <f>SUMPRODUCT($B24:$B26,C24:C26)/SUM($B24:$B26)/10</f>
-        <v>0.93333333333333335</v>
+        <v>1</v>
       </c>
       <c r="D23" s="26"/>
       <c r="E23" s="26"/>
@@ -1544,7 +1544,7 @@
         <v>1</v>
       </c>
       <c r="C25" s="11">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D25" s="11"/>
       <c r="E25" s="11"/>
@@ -1770,7 +1770,7 @@
       </c>
       <c r="C33" s="28">
         <f>((C23*$B23)+(C28*$B28))/$B33</f>
-        <v>0.65833333333333321</v>
+        <v>0.70000000000000007</v>
       </c>
       <c r="D33" s="28"/>
       <c r="E33" s="28"/>
@@ -1849,7 +1849,7 @@
       </c>
       <c r="C36" s="26">
         <f t="shared" ref="C36" si="3">SUMPRODUCT($B37:$B41,C37:C41)/SUM($B37:$B41)/10</f>
-        <v>0.72499999999999998</v>
+        <v>0.4375</v>
       </c>
       <c r="D36" s="26"/>
       <c r="E36" s="26"/>
@@ -1879,7 +1879,7 @@
         <v>2</v>
       </c>
       <c r="C37" s="11">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D37" s="11"/>
       <c r="E37" s="11"/>
@@ -1909,7 +1909,7 @@
         <v>2</v>
       </c>
       <c r="C38" s="11">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D38" s="11"/>
       <c r="E38" s="11"/>
@@ -1939,7 +1939,7 @@
         <v>2</v>
       </c>
       <c r="C39" s="11">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D39" s="11"/>
       <c r="E39" s="11"/>
@@ -1969,7 +1969,7 @@
         <v>1</v>
       </c>
       <c r="C40" s="11">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D40" s="11"/>
       <c r="E40" s="11"/>
@@ -1999,7 +1999,7 @@
         <v>1</v>
       </c>
       <c r="C41" s="11">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D41" s="11"/>
       <c r="E41" s="11"/>
@@ -2163,7 +2163,7 @@
       </c>
       <c r="C47" s="26">
         <f>SUMPRODUCT($B48:$B49,C48:C49)/SUM($B48:$B49)/10</f>
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="D47" s="26"/>
       <c r="E47" s="26"/>
@@ -2193,7 +2193,7 @@
         <v>1</v>
       </c>
       <c r="C48" s="11">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D48" s="11"/>
       <c r="E48" s="11"/>
@@ -2223,7 +2223,7 @@
         <v>1</v>
       </c>
       <c r="C49" s="11">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D49" s="11"/>
       <c r="E49" s="11"/>
@@ -2278,7 +2278,7 @@
       </c>
       <c r="C51" s="28">
         <f>((C36*$B36)+(C43*$B43)+($B47*C47))/$B51</f>
-        <v>0.55499999999999994</v>
+        <v>0.32250000000000001</v>
       </c>
       <c r="D51" s="28"/>
       <c r="E51" s="28"/>
@@ -2333,7 +2333,7 @@
       </c>
       <c r="C53" s="31">
         <f>C20</f>
-        <v>0.93125000000000013</v>
+        <v>0.77499999999999991</v>
       </c>
       <c r="D53" s="31"/>
       <c r="E53" s="31"/>
@@ -2365,7 +2365,7 @@
       </c>
       <c r="C54" s="22">
         <f>C33</f>
-        <v>0.65833333333333321</v>
+        <v>0.70000000000000007</v>
       </c>
       <c r="D54" s="22"/>
       <c r="E54" s="22"/>
@@ -2397,7 +2397,7 @@
       </c>
       <c r="C55" s="22">
         <f t="shared" ref="C55" si="4">C51</f>
-        <v>0.55499999999999994</v>
+        <v>0.32250000000000001</v>
       </c>
       <c r="D55" s="22"/>
       <c r="E55" s="22"/>
@@ -2429,7 +2429,7 @@
       </c>
       <c r="C56" s="13">
         <f t="shared" ref="C56" si="5">SUMPRODUCT($B53:$B55,C53:C55)</f>
-        <v>0.67158333333333331</v>
+        <v>0.56400000000000006</v>
       </c>
       <c r="D56" s="13"/>
       <c r="E56" s="13"/>
@@ -2474,21 +2474,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A9C5319997C6EB4698264EBB41B5521B" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4b6b8c415cc0aea2c8489b5c3bff388a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -2537,10 +2522,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7573310-A6A2-40DF-9EDF-DF83977F74E4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11D559D9-AD8E-43B7-B3C2-03AAE0679091}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2560,16 +2567,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11D559D9-AD8E-43B7-B3C2-03AAE0679091}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7573310-A6A2-40DF-9EDF-DF83977F74E4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>